<commit_message>
Modified excel files and example.ttl, example-abbr.ttl and example-min.ttl to have regions
</commit_message>
<xml_diff>
--- a/examples/WebIndexSimple/structureSimple0.1.xlsx
+++ b/examples/WebIndexSimple/structureSimple0.1.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\computex\examples\WebIndexSimple\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="319" firstSheet="1" activeTab="2"/>
   </bookViews>
@@ -12,12 +17,12 @@
     <sheet name="Countries" sheetId="3" r:id="rId3"/>
     <sheet name="Providers" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="91">
   <si>
     <t>type</t>
   </si>
@@ -163,249 +168,15 @@
     <t>translations...</t>
   </si>
   <si>
-    <t>Argentina</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>Austria</t>
-  </si>
-  <si>
-    <t>Bahrain</t>
-  </si>
-  <si>
-    <t>Bangladesh</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>Benin</t>
-  </si>
-  <si>
-    <t>Botswana</t>
-  </si>
-  <si>
-    <t>Brazil</t>
-  </si>
-  <si>
-    <t>Burkina Faso</t>
-  </si>
-  <si>
-    <t>Cameroon</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
     <t>Chile</t>
   </si>
   <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>Colombia</t>
-  </si>
-  <si>
-    <t>Costa Rica</t>
-  </si>
-  <si>
-    <t>Czech Republic</t>
-  </si>
-  <si>
-    <t>Denmark</t>
-  </si>
-  <si>
-    <t>Ecuador</t>
-  </si>
-  <si>
-    <t>Egypt</t>
-  </si>
-  <si>
-    <t>Estonia</t>
-  </si>
-  <si>
-    <t>Ethiopia</t>
-  </si>
-  <si>
     <t>Finland</t>
   </si>
   <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>Ghana</t>
-  </si>
-  <si>
-    <t>Greece</t>
-  </si>
-  <si>
-    <t>Hungary</t>
-  </si>
-  <si>
-    <t>Iceland</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Indonesia</t>
-  </si>
-  <si>
-    <t>Ireland</t>
-  </si>
-  <si>
-    <t>Israel</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>Jamaica</t>
-  </si>
-  <si>
-    <t>Japan</t>
-  </si>
-  <si>
-    <t>Jordan</t>
-  </si>
-  <si>
-    <t>Kazakhstan</t>
-  </si>
-  <si>
-    <t>Kenya</t>
-  </si>
-  <si>
-    <t>Korea (Rep. of)</t>
-  </si>
-  <si>
-    <t>Malawi</t>
-  </si>
-  <si>
-    <t>Malaysia</t>
-  </si>
-  <si>
-    <t>Mali</t>
-  </si>
-  <si>
-    <t>Mauritius</t>
-  </si>
-  <si>
-    <t>Mexico</t>
-  </si>
-  <si>
-    <t>Morocco</t>
-  </si>
-  <si>
-    <t>Namibia</t>
-  </si>
-  <si>
-    <t>Nepal</t>
-  </si>
-  <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
-    <t>New Zealand</t>
-  </si>
-  <si>
-    <t>Nigeria</t>
-  </si>
-  <si>
-    <t>Norway</t>
-  </si>
-  <si>
-    <t>Pakistan</t>
-  </si>
-  <si>
-    <t>Peru</t>
-  </si>
-  <si>
-    <t>Philippines</t>
-  </si>
-  <si>
-    <t>Poland</t>
-  </si>
-  <si>
-    <t>Portugal</t>
-  </si>
-  <si>
-    <t>Qatar</t>
-  </si>
-  <si>
-    <t>Russia</t>
-  </si>
-  <si>
-    <t>Rwanda</t>
-  </si>
-  <si>
-    <t>Saudi Arabia</t>
-  </si>
-  <si>
-    <t>Senegal</t>
-  </si>
-  <si>
-    <t>Singapore</t>
-  </si>
-  <si>
-    <t>South Africa</t>
-  </si>
-  <si>
     <t>Spain</t>
   </si>
   <si>
-    <t>Sweden</t>
-  </si>
-  <si>
-    <t>Switzerland</t>
-  </si>
-  <si>
-    <t>Tanzania</t>
-  </si>
-  <si>
-    <t>Thailand</t>
-  </si>
-  <si>
-    <t>Tunisia</t>
-  </si>
-  <si>
-    <t>Turkey</t>
-  </si>
-  <si>
-    <t>Uganda</t>
-  </si>
-  <si>
-    <t>United Arab Emirates</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>Uruguay</t>
-  </si>
-  <si>
-    <t>Venezuela</t>
-  </si>
-  <si>
-    <t>Viet Nam</t>
-  </si>
-  <si>
-    <t>Yemen</t>
-  </si>
-  <si>
-    <t>Zambia</t>
-  </si>
-  <si>
-    <t>Zimbabwe</t>
-  </si>
-  <si>
     <t>Website</t>
   </si>
   <si>
@@ -500,6 +271,30 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>Americas</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>FIN</t>
+  </si>
+  <si>
+    <t>ARM</t>
+  </si>
+  <si>
+    <t>ESP</t>
+  </si>
+  <si>
+    <t>CHL</t>
   </si>
 </sst>
 </file>
@@ -567,6 +362,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -614,7 +412,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -649,7 +447,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -918,13 +716,13 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>60</v>
       </c>
       <c r="C2" s="3">
         <v>0.4</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
@@ -932,13 +730,13 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
@@ -960,13 +758,13 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>61</v>
       </c>
       <c r="C5" s="3">
         <v>0.6</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
@@ -974,13 +772,13 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
@@ -988,13 +786,13 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
+        <v>58</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1082,25 +880,25 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>53</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>131</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>159</v>
+        <v>81</v>
       </c>
       <c r="H2" t="s">
-        <v>156</v>
+        <v>78</v>
       </c>
       <c r="L2" t="s">
         <v>34</v>
@@ -1109,68 +907,68 @@
         <v>35</v>
       </c>
       <c r="P2" t="s">
-        <v>144</v>
+        <v>66</v>
       </c>
       <c r="Q2" t="s">
-        <v>148</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>54</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>132</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
-        <v>160</v>
+        <v>82</v>
       </c>
       <c r="H3" t="s">
-        <v>156</v>
+        <v>78</v>
       </c>
       <c r="L3" t="s">
         <v>34</v>
       </c>
       <c r="M3" t="s">
-        <v>137</v>
+        <v>59</v>
       </c>
       <c r="P3" t="s">
-        <v>145</v>
+        <v>67</v>
       </c>
       <c r="Q3" t="s">
-        <v>149</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
-        <v>160</v>
+        <v>82</v>
       </c>
       <c r="H4" t="s">
-        <v>156</v>
+        <v>78</v>
       </c>
       <c r="L4" t="s">
         <v>34</v>
@@ -1179,33 +977,33 @@
         <v>35</v>
       </c>
       <c r="P4" t="s">
-        <v>146</v>
+        <v>68</v>
       </c>
       <c r="Q4" t="s">
-        <v>150</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>56</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>134</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
-        <v>160</v>
+        <v>82</v>
       </c>
       <c r="H5" t="s">
-        <v>156</v>
+        <v>78</v>
       </c>
       <c r="L5" t="s">
         <v>34</v>
@@ -1214,15 +1012,15 @@
         <v>35</v>
       </c>
       <c r="P5" t="s">
-        <v>147</v>
+        <v>69</v>
       </c>
       <c r="Q5" t="s">
-        <v>151</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
@@ -1234,13 +1032,13 @@
         <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>140</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>160</v>
+        <v>82</v>
       </c>
       <c r="H6" t="s">
-        <v>156</v>
+        <v>78</v>
       </c>
       <c r="L6" t="s">
         <v>37</v>
@@ -1249,10 +1047,10 @@
         <v>35</v>
       </c>
       <c r="P6" t="s">
-        <v>142</v>
+        <v>64</v>
       </c>
       <c r="Q6" t="s">
-        <v>152</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1269,13 +1067,13 @@
         <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
       <c r="F7" t="s">
-        <v>160</v>
+        <v>82</v>
       </c>
       <c r="H7" t="s">
-        <v>156</v>
+        <v>78</v>
       </c>
       <c r="L7" t="s">
         <v>37</v>
@@ -1284,10 +1082,10 @@
         <v>35</v>
       </c>
       <c r="P7" t="s">
-        <v>143</v>
+        <v>65</v>
       </c>
       <c r="Q7" t="s">
-        <v>153</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1632,10 +1430,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N82"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1692,408 +1490,47 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
       <c r="B2" t="s">
         <v>48</v>
       </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
       <c r="B3" t="s">
         <v>49</v>
       </c>
+      <c r="C3" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
       <c r="B4" t="s">
         <v>50</v>
       </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
       <c r="B5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="C5" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2130,32 +1567,32 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>130</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>79</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>158</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>